<commit_message>
Note label changed #81
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/potential_ae.xlsx
+++ b/config/itech-aurum/forms/app/potential_ae.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-81\itech-aurum\forms\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD9193D-D6BE-4329-B247-4F8C6A6C60DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4DE734-D2C3-444E-9326-7CAACB306BB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -158,9 +158,6 @@
     <t>../inputs/contact/phone</t>
   </si>
   <si>
-    <t>This form is NOT for AEs recorded in the Day 2 or Day 7 SMS Received forms. Study Nurse will use this form to record every other potential AE report, even if multiple per client, including: 1) A client sends a YES SMS to note a potential AE; 2) A client sends a question about a symptom via SMS; and 3) A client requests a follow-up call.</t>
-  </si>
-  <si>
     <t>select_one days_post_mc</t>
   </si>
   <si>
@@ -396,6 +393,9 @@
   </si>
   <si>
     <t>instance::tag</t>
+  </si>
+  <si>
+    <t>Study Nurse will use this form to record every potential AE reported, even if multiple per client, including: 1) A client sends a YES SMS to note a potential AE; 2) A client sends a question about a symptom via SMS; and 3) A client requests a follow-up call.</t>
   </si>
 </sst>
 </file>
@@ -995,10 +995,10 @@
   <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M26" sqref="M26"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1039,7 +1039,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H1" s="23" t="s">
         <v>6</v>
@@ -1057,7 +1057,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:27">
@@ -1372,15 +1372,15 @@
       <c r="Z13" s="14"/>
       <c r="AA13" s="14"/>
     </row>
-    <row r="14" spans="1:27" ht="99.75">
+    <row r="14" spans="1:27" ht="85.5">
       <c r="A14" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>43</v>
+        <v>122</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
@@ -1395,13 +1395,13 @@
     </row>
     <row r="15" spans="1:27" ht="28.5">
       <c r="A15" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="C15" s="16" t="s">
         <v>45</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>46</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
@@ -1409,7 +1409,7 @@
         <v>39</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="16" spans="1:27" ht="28.5">
       <c r="A16" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="C16" s="16" t="s">
         <v>48</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>49</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
@@ -1434,7 +1434,7 @@
         <v>39</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="16"/>
@@ -1462,13 +1462,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="D17" s="16" t="s">
         <v>51</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>52</v>
       </c>
       <c r="E17" s="16"/>
       <c r="F17" s="16" t="s">
@@ -1498,13 +1498,13 @@
     </row>
     <row r="18" spans="1:27" ht="28.5">
       <c r="A18" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>54</v>
-      </c>
       <c r="C18" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
@@ -1519,13 +1519,13 @@
     </row>
     <row r="19" spans="1:27">
       <c r="A19" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>56</v>
-      </c>
       <c r="C19" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
@@ -1540,13 +1540,13 @@
     </row>
     <row r="20" spans="1:27">
       <c r="A20" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="16" t="s">
         <v>57</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>58</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
@@ -1561,16 +1561,16 @@
     </row>
     <row r="21" spans="1:27">
       <c r="A21" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="C21" s="16" t="s">
+      <c r="D21" s="16" t="s">
         <v>117</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>118</v>
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="16" t="s">
@@ -1589,10 +1589,10 @@
         <v>16</v>
       </c>
       <c r="B22" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="18" t="s">
         <v>59</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>60</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
@@ -1607,13 +1607,13 @@
     </row>
     <row r="23" spans="1:27">
       <c r="A23" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="C23" s="18" t="s">
         <v>62</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>63</v>
       </c>
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
@@ -1631,13 +1631,13 @@
         <v>16</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
@@ -1691,7 +1691,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -1702,35 +1702,35 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1740,79 +1740,79 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1822,29 +1822,29 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
@@ -1855,7 +1855,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1">
         <v>2</v>
@@ -1866,7 +1866,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1">
         <v>3</v>
@@ -1877,7 +1877,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1">
         <v>4</v>
@@ -1888,7 +1888,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="1">
         <v>5</v>
@@ -1899,7 +1899,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" s="1">
         <v>6</v>
@@ -1910,7 +1910,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" s="1">
         <v>7</v>
@@ -1921,7 +1921,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="1">
         <v>8</v>
@@ -1932,7 +1932,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" s="1">
         <v>9</v>
@@ -1943,7 +1943,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" s="1">
         <v>10</v>
@@ -1954,7 +1954,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27" s="1">
         <v>11</v>
@@ -1965,7 +1965,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B28" s="1">
         <v>12</v>
@@ -1976,7 +1976,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29" s="1">
         <v>13</v>
@@ -1987,7 +1987,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" s="1">
         <v>14</v>
@@ -1998,68 +1998,68 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="C36" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C37" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C38" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2089,31 +2089,31 @@
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1">
       <c r="A1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -2135,29 +2135,29 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="C2" s="7">
         <v>43008</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>101</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>

</xml_diff>

<commit_message>
Hiding patient fields, and redoing label change eraged by the merge
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/potential_ae.xlsx
+++ b/config/itech-aurum/forms/app/potential_ae.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-81\itech-aurum\forms\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5772DF1B-3766-490B-92CC-7BE17053C016}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D06A958-FDBA-4325-A085-B392E3C05E41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -164,9 +164,6 @@
     <t>note</t>
   </si>
   <si>
-    <t>This form is NOT for AEs recorded in the Day 2 or Day 7 SMS Received forms. Study Nurse will use this form to record every other potential AE report, even if multiple per client, including: 1) A client sends a YES SMS to note a potential AE; 2) A client sends a question about a symptom via SMS; and 3) A client requests a follow-up call.</t>
-  </si>
-  <si>
     <t>g_post_mc</t>
   </si>
   <si>
@@ -417,6 +414,9 @@
   </si>
   <si>
     <t>instance::tag</t>
+  </si>
+  <si>
+    <t>Study Nurse will use this form to record every potential AE reported, even if multiple per client, including: 1) A client sends a YES SMS to note a potential AE; 2) A client sends a question about a symptom via SMS; and 3) A client requests a follow-up call.</t>
   </si>
 </sst>
 </file>
@@ -1009,10 +1009,10 @@
   <dimension ref="A1:AMJ30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="M13" sqref="M13"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75"/>
@@ -1069,7 +1069,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:27">
@@ -1384,7 +1384,7 @@
       <c r="Z13" s="7"/>
       <c r="AA13" s="7"/>
     </row>
-    <row r="14" spans="1:27" ht="100.5">
+    <row r="14" spans="1:27" ht="86.25">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>44</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -1410,10 +1410,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8" t="s">
@@ -1430,23 +1430,23 @@
     </row>
     <row r="16" spans="1:27" ht="29.25">
       <c r="A16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="C16" s="9" t="s">
         <v>49</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>50</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>30</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -1457,16 +1457,16 @@
     </row>
     <row r="17" spans="1:27">
       <c r="A17" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="C17" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="D17" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="s">
@@ -1502,10 +1502,10 @@
         <v>12</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9" t="s">
@@ -1522,13 +1522,13 @@
     </row>
     <row r="20" spans="1:27" ht="29.25">
       <c r="A20" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="C20" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
@@ -1536,7 +1536,7 @@
         <v>30</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
@@ -1564,13 +1564,13 @@
         <v>17</v>
       </c>
       <c r="B21" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="D21" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9" t="s">
@@ -1631,13 +1631,13 @@
     </row>
     <row r="23" spans="1:27" ht="29.25">
       <c r="A23" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="C23" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>67</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
@@ -1652,13 +1652,13 @@
     </row>
     <row r="24" spans="1:27">
       <c r="A24" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="C24" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>70</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
@@ -1673,13 +1673,13 @@
     </row>
     <row r="25" spans="1:27">
       <c r="A25" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="C25" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>73</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
@@ -1694,16 +1694,16 @@
     </row>
     <row r="26" spans="1:27">
       <c r="A26" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="C26" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="D26" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>77</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="9" t="s">
@@ -1722,10 +1722,10 @@
         <v>17</v>
       </c>
       <c r="B27" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>78</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>79</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
@@ -1740,13 +1740,13 @@
     </row>
     <row r="28" spans="1:27">
       <c r="A28" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B28" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>80</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>81</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
@@ -1764,13 +1764,13 @@
         <v>17</v>
       </c>
       <c r="B29" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="D29" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>84</v>
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
@@ -1822,7 +1822,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>1</v>
@@ -1833,35 +1833,35 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>88</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1871,79 +1871,79 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>90</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>92</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>94</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>96</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>98</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>100</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>102</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1953,29 +1953,29 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B15" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>106</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="17">
         <v>1</v>
@@ -1986,7 +1986,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" s="17">
         <v>2</v>
@@ -1997,7 +1997,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="17">
         <v>3</v>
@@ -2008,7 +2008,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="17">
         <v>4</v>
@@ -2019,7 +2019,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="17">
         <v>5</v>
@@ -2030,7 +2030,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="17">
         <v>6</v>
@@ -2041,7 +2041,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23" s="17">
         <v>7</v>
@@ -2052,7 +2052,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="17">
         <v>8</v>
@@ -2063,7 +2063,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="17">
         <v>9</v>
@@ -2074,7 +2074,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26" s="17">
         <v>10</v>
@@ -2085,7 +2085,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B27" s="17">
         <v>11</v>
@@ -2096,7 +2096,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" s="17">
         <v>12</v>
@@ -2107,7 +2107,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B29" s="17">
         <v>13</v>
@@ -2118,7 +2118,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B30" s="17">
         <v>14</v>
@@ -2129,79 +2129,79 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B31" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>102</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B33" s="17" t="s">
         <v>33</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B37" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" t="s">
         <v>109</v>
-      </c>
-      <c r="C37" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B38" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" t="s">
         <v>111</v>
-      </c>
-      <c r="C38" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B39" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" t="s">
         <v>113</v>
-      </c>
-      <c r="C39" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2227,31 +2227,31 @@
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1">
       <c r="A1" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>119</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>120</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" s="19" t="s">
         <v>121</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>122</v>
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="19"/>
@@ -2273,29 +2273,29 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>123</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>124</v>
       </c>
       <c r="C2" s="23">
         <v>43008</v>
       </c>
       <c r="D2" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>125</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>126</v>
       </c>
       <c r="F2" s="22"/>
       <c r="G2" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2" s="22" t="s">
         <v>127</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>128</v>
       </c>
       <c r="J2" s="22"/>
       <c r="K2" s="22"/>

</xml_diff>

<commit_message>
feat: multi choice followup including photo whatsapp (#829)
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/potential_ae.xlsx
+++ b/config/itech-aurum/forms/app/potential_ae.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D373E6B-5773-DA44-9ACB-D8F6E55CA320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD85A9D-ADA1-D74E-B982-8CD33831A7A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="130">
   <si>
     <t>type</t>
   </si>
@@ -206,9 +206,6 @@
     <t>selected(${symptoms}, 'other')</t>
   </si>
   <si>
-    <t>select_one followup_request</t>
-  </si>
-  <si>
     <t>followup_request</t>
   </si>
   <si>
@@ -405,6 +402,21 @@
   </si>
   <si>
     <t>number</t>
+  </si>
+  <si>
+    <t>photo_review</t>
+  </si>
+  <si>
+    <t>Photo Review</t>
+  </si>
+  <si>
+    <t>whatsapp</t>
+  </si>
+  <si>
+    <t>Whatsapp</t>
+  </si>
+  <si>
+    <t>select_multiple followup_request</t>
   </si>
 </sst>
 </file>
@@ -997,10 +1009,10 @@
   <dimension ref="A1:AMJ29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17:XFD17"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1057,7 +1069,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
@@ -1401,7 +1413,7 @@
         <v>45</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8" t="s">
@@ -1428,7 +1440,7 @@
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>30</v>
@@ -1594,13 +1606,13 @@
     </row>
     <row r="22" spans="1:27" ht="31" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="C22" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -1615,13 +1627,13 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="C23" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
@@ -1636,13 +1648,13 @@
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="C24" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>67</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
@@ -1657,16 +1669,16 @@
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="C25" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="D25" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>71</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="9" t="s">
@@ -1685,10 +1697,10 @@
         <v>17</v>
       </c>
       <c r="B26" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>73</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
@@ -1703,13 +1715,13 @@
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B27" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>74</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>75</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
@@ -1727,13 +1739,13 @@
         <v>17</v>
       </c>
       <c r="B28" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C28" s="11" t="s">
-        <v>77</v>
-      </c>
       <c r="D28" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
@@ -1770,11 +1782,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
+      <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1785,7 +1797,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>1</v>
@@ -1796,35 +1808,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>50</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>81</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1837,10 +1849,10 @@
         <v>53</v>
       </c>
       <c r="B6" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>83</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1848,10 +1860,10 @@
         <v>53</v>
       </c>
       <c r="B7" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>85</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1859,10 +1871,10 @@
         <v>53</v>
       </c>
       <c r="B8" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>87</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1870,10 +1882,10 @@
         <v>53</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>89</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1881,10 +1893,10 @@
         <v>53</v>
       </c>
       <c r="B10" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>91</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1892,10 +1904,10 @@
         <v>53</v>
       </c>
       <c r="B11" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>93</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1903,10 +1915,10 @@
         <v>53</v>
       </c>
       <c r="B12" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>95</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1916,24 +1928,24 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B15" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>99</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2095,76 +2107,98 @@
         <v>47</v>
       </c>
       <c r="B31" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>95</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" s="17" t="s">
         <v>50</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34" s="17" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>101</v>
+        <v>125</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="C37" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="C38" t="s">
-        <v>105</v>
+        <v>80</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B39" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" t="s">
         <v>106</v>
-      </c>
-      <c r="C39" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2190,31 +2224,31 @@
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>112</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>113</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1" s="19" t="s">
         <v>114</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>115</v>
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="19"/>
@@ -2236,29 +2270,29 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>116</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>117</v>
       </c>
       <c r="C2" s="23">
         <v>43008</v>
       </c>
       <c r="D2" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>118</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>119</v>
       </c>
       <c r="F2" s="22"/>
       <c r="G2" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" s="22" t="s">
         <v>120</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>121</v>
       </c>
       <c r="J2" s="22"/>
       <c r="K2" s="22"/>

</xml_diff>

<commit_message>
fix: pae form and report structure and labels
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/potential_ae.xlsx
+++ b/config/itech-aurum/forms/app/potential_ae.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD85A9D-ADA1-D74E-B982-8CD33831A7A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2715E9-77B9-9645-A14A-13121F1E93F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="128">
   <si>
     <t>type</t>
   </si>
@@ -164,27 +164,15 @@
     <t>note</t>
   </si>
   <si>
-    <t>g_post_mc</t>
-  </si>
-  <si>
-    <t>NO_LABEL</t>
-  </si>
-  <si>
     <t>days_post_mc</t>
   </si>
   <si>
-    <t>Day post MC that an AE was reported by client.</t>
-  </si>
-  <si>
     <t>Please select one option</t>
   </si>
   <si>
     <t>text</t>
   </si>
   <si>
-    <t>g_symptoms</t>
-  </si>
-  <si>
     <t>select_multiple  symptoms</t>
   </si>
   <si>
@@ -417,6 +405,12 @@
   </si>
   <si>
     <t>select_multiple followup_request</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Date that a potential AE was reported by client.</t>
   </si>
 </sst>
 </file>
@@ -426,7 +420,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1006,16 +1000,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ29"/>
+  <dimension ref="A1:AMJ25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
       <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="24.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" style="1" customWidth="1"/>
@@ -1031,7 +1025,7 @@
     <col min="13" max="1024" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1069,10 +1063,10 @@
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -1097,7 +1091,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -1122,7 +1116,7 @@
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -1145,7 +1139,7 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1166,7 +1160,7 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="1:27" ht="46" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="46">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1193,7 +1187,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -1214,7 +1208,7 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -1235,7 +1229,7 @@
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27">
       <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
@@ -1252,7 +1246,7 @@
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27">
       <c r="A10" s="3" t="s">
         <v>35</v>
       </c>
@@ -1269,7 +1263,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27">
       <c r="A11" s="5" t="s">
         <v>36</v>
       </c>
@@ -1306,7 +1300,7 @@
       <c r="Z11" s="7"/>
       <c r="AA11" s="7"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -1347,7 +1341,7 @@
       <c r="Z12" s="7"/>
       <c r="AA12" s="7"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -1384,7 +1378,7 @@
       <c r="Z13" s="7"/>
       <c r="AA13" s="7"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="76">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
@@ -1392,7 +1386,7 @@
         <v>44</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -1405,48 +1399,50 @@
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" spans="1:27" ht="76" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="31">
       <c r="A15" s="8" t="s">
-        <v>12</v>
+        <v>126</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-    </row>
-    <row r="16" spans="1:27" ht="31" x14ac:dyDescent="0.2">
+      <c r="C15" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+    </row>
+    <row r="16" spans="1:27" ht="31">
       <c r="A16" s="8" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D16" s="9"/>
-      <c r="E16" s="9" t="s">
-        <v>124</v>
-      </c>
+      <c r="E16" s="9"/>
       <c r="F16" s="9" t="s">
         <v>30</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -1454,16 +1450,38 @@
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="7"/>
+      <c r="AA16" s="7"/>
+    </row>
+    <row r="17" spans="1:27">
       <c r="A17" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
+        <v>17</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="F17" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
@@ -1471,21 +1489,33 @@
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7"/>
+      <c r="AA17" s="7"/>
+    </row>
+    <row r="18" spans="1:27" ht="31">
       <c r="A18" s="8" t="s">
-        <v>12</v>
+        <v>125</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D18" s="9"/>
-      <c r="E18" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
@@ -1495,62 +1525,40 @@
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
     </row>
-    <row r="19" spans="1:27" ht="31" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27">
       <c r="A19" s="8" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
-      <c r="F19" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>55</v>
-      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="7"/>
-      <c r="V19" s="7"/>
-      <c r="W19" s="7"/>
-      <c r="X19" s="7"/>
-      <c r="Y19" s="7"/>
-      <c r="Z19" s="7"/>
-      <c r="AA19" s="7"/>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:27">
       <c r="A20" s="8" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>58</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="D20" s="9"/>
       <c r="E20" s="9"/>
-      <c r="F20" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
@@ -1558,30 +1566,24 @@
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="7"/>
-      <c r="V20" s="7"/>
-      <c r="W20" s="7"/>
-      <c r="X20" s="7"/>
-      <c r="Y20" s="7"/>
-      <c r="Z20" s="7"/>
-      <c r="AA20" s="7"/>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:27">
       <c r="A21" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
+        <v>63</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>66</v>
+      </c>
       <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
+      <c r="F21" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
@@ -1589,190 +1591,88 @@
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
-      <c r="U21" s="7"/>
-      <c r="V21" s="7"/>
-      <c r="W21" s="7"/>
-      <c r="X21" s="7"/>
-      <c r="Y21" s="7"/>
-      <c r="Z21" s="7"/>
-      <c r="AA21" s="7"/>
-    </row>
-    <row r="22" spans="1:27" ht="31" x14ac:dyDescent="0.2">
-      <c r="A22" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="9" t="s">
+    </row>
+    <row r="22" spans="1:27">
+      <c r="A22" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+    </row>
+    <row r="23" spans="1:27">
+      <c r="A23" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A23" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A25" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="9" t="s">
+      <c r="B23" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="C23" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+    </row>
+    <row r="24" spans="1:27">
+      <c r="A24" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B24" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C24" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
+      <c r="D24" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+    </row>
+    <row r="25" spans="1:27">
+      <c r="A25" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1789,15 +1689,15 @@
       <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>1</v>
@@ -1806,151 +1706,151 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="17"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B6" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C8" s="17" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="17" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C9" s="17" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="17" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C10" s="17" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="17" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C11" s="17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="17" t="s">
+    <row r="12" spans="1:3">
+      <c r="A12" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C12" s="17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" s="17" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="17" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B17" s="17">
         <v>1</v>
@@ -1959,9 +1859,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B18" s="17">
         <v>2</v>
@@ -1970,9 +1870,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B19" s="17">
         <v>3</v>
@@ -1981,9 +1881,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B20" s="17">
         <v>4</v>
@@ -1992,9 +1892,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B21" s="17">
         <v>5</v>
@@ -2003,9 +1903,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B22" s="17">
         <v>6</v>
@@ -2014,9 +1914,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B23" s="17">
         <v>7</v>
@@ -2025,9 +1925,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B24" s="17">
         <v>8</v>
@@ -2036,9 +1936,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B25" s="17">
         <v>9</v>
@@ -2047,9 +1947,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B26" s="17">
         <v>10</v>
@@ -2058,9 +1958,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B27" s="17">
         <v>11</v>
@@ -2069,9 +1969,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B28" s="17">
         <v>12</v>
@@ -2080,9 +1980,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3">
       <c r="A29" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B29" s="17">
         <v>13</v>
@@ -2091,9 +1991,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3">
       <c r="A30" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B30" s="17">
         <v>14</v>
@@ -2102,103 +2002,103 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3">
       <c r="A31" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>50</v>
-      </c>
       <c r="C33" s="17" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B34" s="17" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C37" s="18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="17" t="s">
+    <row r="41" spans="1:3">
+      <c r="A41" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C41" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="C40" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="C41" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2213,7 +2113,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="2" width="43.6640625" customWidth="1"/>
@@ -2222,33 +2122,33 @@
     <col min="16" max="26" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="18" customHeight="1">
       <c r="A1" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>108</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>112</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="19"/>
@@ -2268,31 +2168,31 @@
       <c r="Y1" s="20"/>
       <c r="Z1" s="20"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="21" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C2" s="23">
         <v>43008</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F2" s="22"/>
       <c r="G2" s="22" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="J2" s="22"/>
       <c r="K2" s="22"/>

</xml_diff>

<commit_message>
feat: change PAE question  flow
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/potential_ae.xlsx
+++ b/config/itech-aurum/forms/app/potential_ae.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2715E9-77B9-9645-A14A-13121F1E93F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA46B891-6364-6043-A8AB-03F5646CAE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -167,9 +167,6 @@
     <t>days_post_mc</t>
   </si>
   <si>
-    <t>Please select one option</t>
-  </si>
-  <si>
     <t>text</t>
   </si>
   <si>
@@ -411,6 +408,9 @@
   </si>
   <si>
     <t>Date that a potential AE was reported by client.</t>
+  </si>
+  <si>
+    <t>. &lt;= date(today()) and . &gt;= date(today() - 28)</t>
   </si>
 </sst>
 </file>
@@ -1000,13 +1000,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ25"/>
+  <dimension ref="A1:AMJ26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
@@ -1018,7 +1018,7 @@
     <col min="5" max="5" width="9.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.5" style="1"/>
     <col min="7" max="7" width="19.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5" style="1"/>
+    <col min="8" max="8" width="32.83203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="34" style="1" customWidth="1"/>
     <col min="10" max="11" width="11.5" style="1"/>
     <col min="12" max="12" width="20.1640625" style="1" customWidth="1"/>
@@ -1063,7 +1063,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:27">
@@ -1386,7 +1386,7 @@
         <v>44</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -1401,88 +1401,70 @@
     </row>
     <row r="15" spans="1:27" ht="31">
       <c r="A15" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9" t="s">
+        <v>127</v>
+      </c>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:27" ht="31">
-      <c r="A16" s="8" t="s">
+    <row r="16" spans="1:27">
+      <c r="A16" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+    </row>
+    <row r="17" spans="1:27" ht="31">
+      <c r="A17" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="C17" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
-      <c r="W16" s="7"/>
-      <c r="X16" s="7"/>
-      <c r="Y16" s="7"/>
-      <c r="Z16" s="7"/>
-      <c r="AA16" s="7"/>
-    </row>
-    <row r="17" spans="1:27">
-      <c r="A17" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="9"/>
+      <c r="G17" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
@@ -1504,19 +1486,23 @@
       <c r="Z17" s="7"/>
       <c r="AA17" s="7"/>
     </row>
-    <row r="18" spans="1:27" ht="31">
+    <row r="18" spans="1:27">
       <c r="A18" s="8" t="s">
-        <v>125</v>
+        <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="9"/>
+        <v>52</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="F18" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -1524,16 +1510,30 @@
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
-    </row>
-    <row r="19" spans="1:27">
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7"/>
+    </row>
+    <row r="19" spans="1:27" ht="31">
       <c r="A19" s="8" t="s">
-        <v>57</v>
+        <v>124</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -1548,13 +1548,13 @@
     </row>
     <row r="20" spans="1:27">
       <c r="A20" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
@@ -1569,21 +1569,17 @@
     </row>
     <row r="21" spans="1:27">
       <c r="A21" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>66</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="D21" s="9"/>
       <c r="E21" s="9"/>
-      <c r="F21" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
@@ -1593,35 +1589,39 @@
       <c r="M21" s="9"/>
     </row>
     <row r="22" spans="1:27">
-      <c r="A22" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
+      <c r="A22" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
     </row>
     <row r="23" spans="1:27">
       <c r="A23" s="10" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
@@ -1634,45 +1634,45 @@
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:27">
-      <c r="A24" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-    </row>
     <row r="25" spans="1:27">
       <c r="A25" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+    </row>
+    <row r="26" spans="1:27">
+      <c r="A26" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1697,7 +1697,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>1</v>
@@ -1708,35 +1708,35 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>76</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1746,79 +1746,79 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>78</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>80</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>82</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>84</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>86</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>88</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>90</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1828,24 +1828,24 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B15" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>94</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2007,98 +2007,98 @@
         <v>45</v>
       </c>
       <c r="B31" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>90</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B34" s="17" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B35" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C35" s="17" t="s">
         <v>121</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B36" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" s="17" t="s">
         <v>123</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B39" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" t="s">
         <v>97</v>
-      </c>
-      <c r="C39" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B40" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" t="s">
         <v>99</v>
-      </c>
-      <c r="C40" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B41" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" t="s">
         <v>101</v>
-      </c>
-      <c r="C41" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2124,31 +2124,31 @@
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1">
       <c r="A1" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>107</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>108</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" s="19" t="s">
         <v>109</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>110</v>
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="19"/>
@@ -2170,29 +2170,29 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>111</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>112</v>
       </c>
       <c r="C2" s="23">
         <v>43008</v>
       </c>
       <c r="D2" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>113</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>114</v>
       </c>
       <c r="F2" s="22"/>
       <c r="G2" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="22" t="s">
         <v>115</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>116</v>
       </c>
       <c r="J2" s="22"/>
       <c r="K2" s="22"/>

</xml_diff>

<commit_message>
feat: update client review title
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/potential_ae.xlsx
+++ b/config/itech-aurum/forms/app/potential_ae.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD85A9D-ADA1-D74E-B982-8CD33831A7A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75ED12A2-D1B4-244B-B16F-C609FA4EAABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="25600" windowHeight="15500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -374,9 +374,6 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>Received SMS: potential AE</t>
-  </si>
-  <si>
     <t>potential_ae</t>
   </si>
   <si>
@@ -417,6 +414,9 @@
   </si>
   <si>
     <t>select_multiple followup_request</t>
+  </si>
+  <si>
+    <t>Received SMS: Potential AE</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -597,33 +597,32 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="8" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1008,7 +1007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
@@ -1069,7 +1068,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
@@ -1413,7 +1412,7 @@
         <v>45</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8" t="s">
@@ -1440,7 +1439,7 @@
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>30</v>
@@ -1606,7 +1605,7 @@
     </row>
     <row r="22" spans="1:27" ht="31" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>59</v>
@@ -1745,7 +1744,7 @@
         <v>76</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
@@ -2140,10 +2139,10 @@
         <v>59</v>
       </c>
       <c r="B35" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="17" t="s">
         <v>125</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -2151,10 +2150,10 @@
         <v>59</v>
       </c>
       <c r="B36" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C36" s="17" t="s">
         <v>127</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -2211,7 +2210,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2270,47 +2271,29 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="22">
+        <v>43008</v>
+      </c>
+      <c r="D2" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="23">
-        <v>43008</v>
-      </c>
-      <c r="D2" s="22" t="s">
+      <c r="E2" t="s">
         <v>117</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="G2" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22" t="s">
+      <c r="H2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I2" t="s">
         <v>119</v>
       </c>
-      <c r="H2" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>